<commit_message>
basic upload file of dosage form group complete
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/files/dosageformgroup_template.xlsx
+++ b/src/main/webapp/resources/files/dosageformgroup_template.xlsx
@@ -1,25 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\company\project-source-code\drug-catalog\src\main\webapp\resources\files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11412"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
@@ -32,19 +22,19 @@
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>ID ควรเป็นตัวอักษรเล็กทั้งหมด และห้ามปล่อยว่างไว้</t>
-  </si>
-  <si>
     <t>injection</t>
   </si>
   <si>
-    <t>อัดฉีด</t>
-  </si>
-  <si>
     <t>powder</t>
   </si>
   <si>
-    <t>ผง</t>
+    <t>แบบฉีดเข้าเส้นเลือด</t>
+  </si>
+  <si>
+    <t>แบบผงกรอก</t>
+  </si>
+  <si>
+    <t>ID ห้ามเป็นค่าว่าง และเป็นตัวพิมพ์เล็กทั้งหมด</t>
   </si>
 </sst>
 </file>
@@ -80,14 +70,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -110,39 +101,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,157 +212,181 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" customWidth="1"/>
-    <col min="2" max="2" width="26.21875" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -384,22 +399,25 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
basic validate dosageformgroup upload excel
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/files/dosageformgroup_template.xlsx
+++ b/src/main/webapp/resources/files/dosageformgroup_template.xlsx
@@ -34,7 +34,7 @@
     <t>แบบผงกรอก</t>
   </si>
   <si>
-    <t>ID ห้ามเป็นค่าว่าง และเป็นตัวพิมพ์เล็กทั้งหมด</t>
+    <t>ID ห้ามเป็นค่าว่าง และเป็นตัวพิมพ์เล็กทั้งหมด และต้องขึ้นต้นด้วยตัวอักษร a-z เท่านั้น</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
upload mapped tmt and dosage form group complete
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/files/dosageformgroup_template.xlsx
+++ b/src/main/webapp/resources/files/dosageformgroup_template.xlsx
@@ -1,40 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14388" windowHeight="4836"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>DESCRIPTION</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+  <si>
+    <t>DOSAGE_FORM_GROUP จะต้องมีอยู่แล้วในฐานข้อมูล</t>
+  </si>
+  <si>
+    <t>DOSAGE_FORM_GROUP ห้ามเป็นค่าว่าง และเป็นตัวพิมพ์เล็กทั้งหมด และต้องขึ้นต้นด้วยตัวอักษร a-z เท่านั้น</t>
   </si>
   <si>
     <t>injection</t>
   </si>
   <si>
-    <t>powder</t>
-  </si>
-  <si>
-    <t>แบบฉีดเข้าเส้นเลือด</t>
-  </si>
-  <si>
-    <t>แบบผงกรอก</t>
-  </si>
-  <si>
-    <t>ID ห้ามเป็นค่าว่าง และเป็นตัวพิมพ์เล็กทั้งหมด และต้องขึ้นต้นด้วยตัวอักษร a-z เท่านั้น</t>
+    <t>TMTID ห้ามเป็นค่าว่าง</t>
+  </si>
+  <si>
+    <t>DOSAGE_FORM_GROUP</t>
+  </si>
+  <si>
+    <t>TMTID</t>
   </si>
 </sst>
 </file>
@@ -70,15 +77,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -101,39 +111,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -212,166 +222,142 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
@@ -380,46 +366,58 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="30.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2">
+        <v>100005</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="A3" s="2">
+        <v>100014</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
+      <c r="A4" s="2">
+        <v>513262</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>